<commit_message>
[Pipette] MP2 data update
</commit_message>
<xml_diff>
--- a/0_MP2 Data/Pipette Change list MP2.xlsx
+++ b/0_MP2 Data/Pipette Change list MP2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554B5B9C-5DDF-4976-8C1F-36BBF3FA1A0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252D4933-12AB-409F-AF56-E92B468866B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +144,86 @@
   </si>
   <si>
     <t>Gate Decal 수정 및 Pin re-assign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCH&amp;PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BZT52C5V1S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Off 안되는 문제 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.7uF/25V 1608</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S1M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset시 S/V On 상태 유지하는 문제 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1N4148WS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V Not operation 개선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB 수정 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board Cut out 영역 축소-Bobbin에 맞춰 조정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FET Gate에 shunt R 10K 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery Silk line 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buck Enable Pin에 Pull-Down R 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -151,7 +231,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +255,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -190,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -452,11 +541,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,6 +630,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,12 +665,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -806,10 +956,467 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.796875" customWidth="1"/>
+    <col min="2" max="2" width="5.19921875" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.09765625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="36.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:9" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37">
+        <v>43460</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="36"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="36"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B10" s="12">
+        <v>8</v>
+      </c>
+      <c r="C10" s="32">
+        <v>43478</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B11" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="31"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B12" s="12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="32">
+        <v>43480</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="27">
+        <v>100</v>
+      </c>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B15" s="12">
+        <v>13</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B16" s="12">
+        <v>14</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B17" s="12">
+        <v>15</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B18" s="12">
+        <v>16</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B19" s="12">
+        <v>17</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B20" s="12">
+        <v>18</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B21" s="12">
+        <v>19</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B22" s="12">
+        <v>20</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="26"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="26"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="C3:C9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C10:C12"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D1006C-F734-43AF-9925-FD425A6F32B4}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -850,22 +1457,22 @@
       <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="37">
         <v>43460</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="38" t="s">
         <v>11</v>
       </c>
     </row>
@@ -873,12 +1480,12 @@
       <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
@@ -886,18 +1493,18 @@
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="24"/>
+      <c r="H4" s="39"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
@@ -905,85 +1512,77 @@
       <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="24"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="24"/>
+        <v>30</v>
+      </c>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" s="12">
         <v>7</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>24</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" s="12">
@@ -993,255 +1592,9 @@
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B11" s="12">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B12" s="14"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B13" s="14"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B15" s="14"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="18"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="C3:C9"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D1006C-F734-43AF-9925-FD425A6F32B4}">
-  <dimension ref="B1:H16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="4.796875" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.09765625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="36.69921875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25">
-        <v>43460</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B4" s="12">
-        <v>2</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B5" s="12">
-        <v>3</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B6" s="12">
-        <v>4</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B7" s="12">
-        <v>5</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="12">
-        <v>6</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="22"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="12">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B10" s="12">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
[Pipette] V3.0 SCH,PCB,BOM 수정
</commit_message>
<xml_diff>
--- a/0_MP2 Data/Pipette Change list MP2.xlsx
+++ b/0_MP2 Data/Pipette Change list MP2.xlsx
@@ -1,242 +1,294 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252D4933-12AB-409F-AF56-E92B468866B0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Trans" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reference</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Before</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>After</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>COMMENT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>J3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>GND PAD에 VIA 4ea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>PAD Side로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>PCB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SMT 개선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>J1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>GND PAD에 VIA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SW1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>+3.3V PAD에 VIA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>U4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>V_BATT PAD에 VIA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>D2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SCH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Q3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>PMBT2222</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>FTK2306</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>S/V Not operation 개선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Q1,Q2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Board Cut out 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TX1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Gate Decal 수정 및 Pin re-assign</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SCH&amp;PCB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>D5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Off 안되는 문제 개선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.7uF/25V 1608</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S1M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset시 S/V On 상태 유지하는 문제 개선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1N4148WS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10K</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V Not operation 개선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board Cut out 영역 축소-Bobbin에 맞춰 조정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FET Gate에 shunt R 10K 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery Silk line 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buck Enable Pin에 Pull-Down R 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>BZT52C5V1S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plasma Off 안되는 문제 개선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.7uF/25V 1608</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S1M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reset시 S/V On 상태 유지하는 문제 개선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1N4148WS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BATT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MOLEX5268-02P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>053048-0210</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3A 지원 CON로 변경</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>U4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LM2735XMF</t>
+  </si>
+  <si>
+    <t>LM2735XSD</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHIP 발열 개선을 위해 Package 변경</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R35</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R31</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>R34</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10K</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S/V Not operation 개선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCB 수정 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Board Cut out 영역 축소-Bobbin에 맞춰 조정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FET Gate에 shunt R 10K 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Battery Silk line 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Buck Enable Pin에 Pull-Down R 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,15 +309,157 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +472,187 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -580,16 +953,276 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -601,7 +1234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,7 +1242,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -618,38 +1251,85 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="1" xfId="33" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -658,15 +1338,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,18 +1347,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="52">
+    <cellStyle name="20% - 강조색1" xfId="16" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색2" xfId="19" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색3" xfId="22" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색4" xfId="25" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색5" xfId="28" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색6" xfId="31" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색1" xfId="17" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색2" xfId="20" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색3" xfId="23" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색4" xfId="26" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색5" xfId="29" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색6" xfId="32" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 강조색1 2" xfId="45"/>
+    <cellStyle name="60% - 강조색1 3" xfId="37"/>
+    <cellStyle name="60% - 강조색2 2" xfId="46"/>
+    <cellStyle name="60% - 강조색2 3" xfId="38"/>
+    <cellStyle name="60% - 강조색3 2" xfId="47"/>
+    <cellStyle name="60% - 강조색3 3" xfId="39"/>
+    <cellStyle name="60% - 강조색4 2" xfId="48"/>
+    <cellStyle name="60% - 강조색4 3" xfId="40"/>
+    <cellStyle name="60% - 강조색5 2" xfId="49"/>
+    <cellStyle name="60% - 강조색5 3" xfId="41"/>
+    <cellStyle name="60% - 강조색6 2" xfId="50"/>
+    <cellStyle name="60% - 강조색6 3" xfId="42"/>
+    <cellStyle name="강조색1" xfId="15" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="강조색2" xfId="18" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="강조색3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="강조색4" xfId="24" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="강조색5" xfId="27" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="강조색6" xfId="30" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="경고문" xfId="12" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="계산" xfId="9" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="나쁨" xfId="6" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="메모 2" xfId="36"/>
+    <cellStyle name="보통 2" xfId="44"/>
+    <cellStyle name="보통 3" xfId="35"/>
+    <cellStyle name="설명 텍스트" xfId="13" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="셀 확인" xfId="11" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="쉼표 [0] 2" xfId="51"/>
+    <cellStyle name="쉼표 [0] 3" xfId="43"/>
+    <cellStyle name="연결된 셀" xfId="10" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="요약" xfId="14" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="입력" xfId="7" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="제목 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="제목 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="제목 3" xfId="3" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="제목 4" xfId="4" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="제목 5" xfId="34"/>
+    <cellStyle name="좋음" xfId="5" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="출력" xfId="8" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="33"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -948,32 +1675,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.796875" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.09765625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="36.69921875" customWidth="1"/>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="5.25" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="36.75" customWidth="1"/>
+    <col min="8" max="8" width="12.875" customWidth="1"/>
+    <col min="9" max="9" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:9" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -992,445 +1721,534 @@
       <c r="G2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B3" s="8">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="59">
         <v>1</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="50">
         <v>43460</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B4" s="12">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="60">
         <v>2</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="36"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B5" s="12">
+      <c r="H4" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="49"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="60">
         <v>3</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="36"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B6" s="12">
+      <c r="H5" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="49"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="60">
         <v>4</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="36"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B7" s="12">
+      <c r="H6" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="49"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="60">
         <v>5</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="36"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B8" s="12">
+      <c r="H7" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="49"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="60">
         <v>6</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="47"/>
+      <c r="D8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="36"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B9" s="12">
+      <c r="H8" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="49"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="60">
         <v>7</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B10" s="12">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="60">
         <v>8</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="42">
         <v>43478</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="60">
+        <v>9</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="46"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="60">
+        <v>10</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B11" s="12">
-        <v>9</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="3" t="s">
+      <c r="F12" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="60">
+        <v>11</v>
+      </c>
+      <c r="C13" s="42">
+        <v>43480</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E13" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="60">
+        <v>12</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="35">
+        <v>100</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="45"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="60">
+        <v>13</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="60">
+        <v>14</v>
+      </c>
+      <c r="C16" s="42">
+        <v>43522</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="60">
+        <v>15</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="60">
+        <v>16</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="31"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B12" s="12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B13" s="12">
-        <v>11</v>
-      </c>
-      <c r="C13" s="32">
-        <v>43480</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="28" t="s">
+      <c r="G18" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B14" s="12">
-        <v>12</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="27">
-        <v>100</v>
-      </c>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B15" s="12">
-        <v>13</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B16" s="12">
-        <v>14</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B17" s="12">
-        <v>15</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" s="12">
-        <v>16</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="26"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>17</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
-      <c r="H19" s="26"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H19" s="25"/>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="12">
         <v>18</v>
       </c>
-      <c r="C20" s="24"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="26"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="G20" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>19</v>
       </c>
-      <c r="C21" s="24"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
-      <c r="H21" s="26"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H21" s="25"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <v>20</v>
       </c>
-      <c r="C22" s="24"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
       <c r="F22" s="24"/>
       <c r="G22" s="24"/>
-      <c r="H22" s="26"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H22" s="25"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
-      <c r="H23" s="26"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
       <c r="D24" s="25"/>
       <c r="E24" s="25"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
-      <c r="H24" s="26"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
-      <c r="H25" s="26"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H25" s="25"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="23"/>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
-      <c r="H26" s="26"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H26" s="25"/>
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="23"/>
       <c r="C27" s="24"/>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="26"/>
-    </row>
-    <row r="28" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H27" s="25"/>
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="15"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
-      <c r="H28" s="18"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H13:H15"/>
+  <mergeCells count="7">
+    <mergeCell ref="I13:I15"/>
     <mergeCell ref="C13:C15"/>
-    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="I3:I8"/>
     <mergeCell ref="C3:C9"/>
-    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
     <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C16:C18"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D1006C-F734-43AF-9925-FD425A6F32B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.796875" customWidth="1"/>
-    <col min="2" max="2" width="5.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.09765625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="36.69921875" customWidth="1"/>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="5.25" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:8" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1453,11 +2271,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="51">
         <v>43460</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -1472,15 +2290,15 @@
       <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="54" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1493,13 +2311,13 @@
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="39"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H4" s="55"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1512,13 +2330,13 @@
       <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H5" s="55"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1531,13 +2349,13 @@
       <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="40"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H6" s="56"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1552,11 +2370,11 @@
       </c>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +2389,7 @@
       </c>
       <c r="H8" s="22"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -1580,11 +2398,11 @@
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
         <v>8</v>
       </c>
@@ -1593,11 +2411,11 @@
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>9</v>
       </c>
@@ -1608,7 +2426,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
@@ -1617,7 +2435,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="7"/>
       <c r="D13" s="3"/>
@@ -1626,7 +2444,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="7"/>
       <c r="D14" s="3"/>
@@ -1635,7 +2453,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
@@ -1644,7 +2462,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
@@ -1658,7 +2476,7 @@
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="H3:H6"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[MP2] MP2 Trans data 작업 및 Release
</commit_message>
<xml_diff>
--- a/0_MP2 Data/Pipette Change list MP2.xlsx
+++ b/0_MP2 Data/Pipette Change list MP2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="72">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -298,6 +298,10 @@
   <si>
     <t>KEY_OP RC filter 추가
 Key 인식 문제시 tune</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cutting line 표시</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1250,7 +1254,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1393,6 +1397,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1715,7 +1722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2312,7 +2319,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2471,8 +2478,12 @@
       <c r="B9" s="12">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="64">
+        <v>43530</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
@@ -2484,11 +2495,15 @@
       <c r="B10" s="12">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -2548,9 +2563,10 @@
       <c r="H16" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="H3:H6"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[MP2]Main PCB 수정 - 기구 사항 반영
</commit_message>
<xml_diff>
--- a/0_MP2 Data/Pipette Change list MP2.xlsx
+++ b/0_MP2 Data/Pipette Change list MP2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -302,6 +302,38 @@
   </si>
   <si>
     <t>Cutting line 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/14 기구 도면 반영</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>외곽 형상 및 CON 위치 변경</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>J1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC-011C_SMD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -689,7 +721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1097,6 +1129,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1254,7 +1310,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1325,9 +1381,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1402,6 +1455,35 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="20% - 강조색1" xfId="16" builtinId="30" customBuiltin="1"/>
@@ -1722,7 +1804,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1733,7 +1815,7 @@
   <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1776,10 +1858,10 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="44">
+      <c r="B3" s="43">
         <v>1</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="49">
         <v>43460</v>
       </c>
       <c r="D3" s="27" t="s">
@@ -1794,18 +1876,18 @@
       <c r="G3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="47" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="45">
+      <c r="B4" s="44">
         <v>2</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="30" t="s">
         <v>10</v>
       </c>
@@ -1818,16 +1900,16 @@
       <c r="G4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="49"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="45">
+      <c r="B5" s="44">
         <v>3</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="30" t="s">
         <v>10</v>
       </c>
@@ -1840,16 +1922,16 @@
       <c r="G5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="49"/>
+      <c r="I5" s="48"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <v>4</v>
       </c>
-      <c r="C6" s="51"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="30" t="s">
         <v>10</v>
       </c>
@@ -1862,16 +1944,16 @@
       <c r="G6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="49"/>
+      <c r="I6" s="48"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <v>5</v>
       </c>
-      <c r="C7" s="51"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="30" t="s">
         <v>10</v>
       </c>
@@ -1884,16 +1966,16 @@
       <c r="G7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="49"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>6</v>
       </c>
-      <c r="C8" s="51"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="30" t="s">
         <v>10</v>
       </c>
@@ -1906,16 +1988,16 @@
       <c r="G8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="49"/>
+      <c r="I8" s="48"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>7</v>
       </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="51"/>
       <c r="D9" s="30" t="s">
         <v>20</v>
       </c>
@@ -1928,7 +2010,7 @@
       <c r="G9" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="36" t="s">
         <v>59</v>
       </c>
       <c r="I9" s="34" t="s">
@@ -1936,10 +2018,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>8</v>
       </c>
-      <c r="C10" s="55">
+      <c r="C10" s="54">
         <v>43478</v>
       </c>
       <c r="D10" s="30" t="s">
@@ -1954,18 +2036,18 @@
       <c r="G10" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="52" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="45">
+      <c r="B11" s="44">
         <v>9</v>
       </c>
-      <c r="C11" s="51"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="30" t="s">
         <v>31</v>
       </c>
@@ -1978,16 +2060,16 @@
       <c r="G11" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="54"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="45">
+      <c r="B12" s="44">
         <v>10</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="30" t="s">
         <v>31</v>
       </c>
@@ -2000,7 +2082,7 @@
       <c r="G12" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="42" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="34" t="s">
@@ -2008,10 +2090,10 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="45">
+      <c r="B13" s="44">
         <v>11</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="54">
         <v>43480</v>
       </c>
       <c r="D13" s="30" t="s">
@@ -2026,18 +2108,18 @@
       <c r="G13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="I13" s="52" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="45">
+      <c r="B14" s="44">
         <v>12</v>
       </c>
-      <c r="C14" s="51"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="30" t="s">
         <v>20</v>
       </c>
@@ -2050,16 +2132,16 @@
       <c r="G14" s="35">
         <v>100</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="57"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="45">
+      <c r="B15" s="44">
         <v>13</v>
       </c>
-      <c r="C15" s="52"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="30" t="s">
         <v>31</v>
       </c>
@@ -2072,200 +2154,234 @@
       <c r="G15" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I15" s="54"/>
+      <c r="I15" s="53"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="45">
+      <c r="B16" s="44">
         <v>14</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="54">
         <v>43522</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="I16" s="38" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="45">
+      <c r="B17" s="44">
         <v>15</v>
       </c>
-      <c r="C17" s="51"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="38" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="45">
+      <c r="B18" s="44">
         <v>16</v>
       </c>
-      <c r="C18" s="52"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="36" t="s">
         <v>55</v>
       </c>
       <c r="F18" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="37" t="s">
+      <c r="H18" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="37" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="45">
+      <c r="B19" s="44">
         <v>17</v>
       </c>
-      <c r="C19" s="55">
+      <c r="C19" s="54">
         <v>43526</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="38" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="45">
+      <c r="B20" s="44">
         <v>18</v>
       </c>
-      <c r="C20" s="51"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="46">
         <v>0</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="56" t="s">
+      <c r="I20" s="55" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="45">
+    <row r="21" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="64">
         <v>19</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="30" t="s">
+      <c r="C21" s="50"/>
+      <c r="D21" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="54"/>
+      <c r="I21" s="56"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="12">
+      <c r="B22" s="43">
         <v>20</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24" t="s">
+      <c r="C22" s="49">
+        <v>43540</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="73" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="44">
+        <v>21</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="74">
+        <v>22</v>
+      </c>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26"/>
+      <c r="H24" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="23"/>
@@ -2298,7 +2414,8 @@
       <c r="I28" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="C22:C24"/>
     <mergeCell ref="I3:I8"/>
     <mergeCell ref="C3:C9"/>
     <mergeCell ref="I10:I11"/>
@@ -2319,7 +2436,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2360,7 +2477,7 @@
       <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>43460</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -2375,7 +2492,7 @@
       <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="60" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2383,7 +2500,7 @@
       <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
@@ -2396,13 +2513,13 @@
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="62"/>
+      <c r="H4" s="61"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="59"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2415,13 +2532,13 @@
       <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="62"/>
+      <c r="H5" s="61"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="59"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -2434,13 +2551,13 @@
       <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="C7" s="59"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2459,7 +2576,7 @@
       <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="C8" s="60"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
@@ -2478,7 +2595,7 @@
       <c r="B9" s="12">
         <v>7</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="63">
         <v>43530</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2495,7 +2612,7 @@
       <c r="B10" s="12">
         <v>8</v>
       </c>
-      <c r="C10" s="60"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>